<commit_message>
documentation: example 2 aggregate events
</commit_message>
<xml_diff>
--- a/example/my_file.xlsx
+++ b/example/my_file.xlsx
@@ -233,67 +233,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-0.004692317645432618</c:v>
+                  <c:v>-0.003935650435941625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.002418608446780616</c:v>
+                  <c:v>0.005950448806269467</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0005499380464074931</c:v>
+                  <c:v>0.04281994191779238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.870876876734848e-05</c:v>
+                  <c:v>0.04674959426742286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.003895047376566452</c:v>
+                  <c:v>0.03183356624277132</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.02962631045493755</c:v>
+                  <c:v>0.02388374645065854</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.05450309544596235</c:v>
+                  <c:v>0.01703507856115128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.06555623092573601</c:v>
+                  <c:v>0.007150699977886603</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.05022903251722063</c:v>
+                  <c:v>0.007236195209396145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.05593573581763552</c:v>
+                  <c:v>0.003172527907350148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.07713944736617602</c:v>
+                  <c:v>0.004072387906190416</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08447724494719333</c:v>
+                  <c:v>-0.005879888339812385</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.08721244242613338</c:v>
+                  <c:v>-0.02204370693072761</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.09244775083851461</c:v>
+                  <c:v>-0.01314380760183279</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.09292141277758562</c:v>
+                  <c:v>-0.005694785216119432</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.08515191877092428</c:v>
+                  <c:v>-8.130602839034103e-05</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.07900849891684136</c:v>
+                  <c:v>-0.003652785340608557</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0649611656058684</c:v>
+                  <c:v>-0.01242499502594216</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.05561027686300996</c:v>
+                  <c:v>-0.007141633021236225</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.05768679968751465</c:v>
+                  <c:v>-0.009074582198673804</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.05393362031670209</c:v>
+                  <c:v>-0.008380877714481261</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,67 +404,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-0.004692317645432618</c:v>
+                  <c:v>-0.003935650435941625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.002273709198652002</c:v>
+                  <c:v>0.009886099242211092</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.002968546493188109</c:v>
+                  <c:v>0.03686949311152292</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0005312292776401446</c:v>
+                  <c:v>0.003929652349630477</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.003876338607799104</c:v>
+                  <c:v>-0.01491602802465154</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0257312630783711</c:v>
+                  <c:v>-0.00794981979211278</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.02487678499102481</c:v>
+                  <c:v>-0.006848667889507258</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.01105313547977366</c:v>
+                  <c:v>-0.009884378583264674</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.01532719840851537</c:v>
+                  <c:v>8.549523150954211e-05</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.005706703300414887</c:v>
+                  <c:v>-0.004063667302045998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0212037115485405</c:v>
+                  <c:v>0.000899859998840269</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.007337797581017312</c:v>
+                  <c:v>-0.009952276246002801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.002735197478940056</c:v>
+                  <c:v>-0.01616381859091522</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.005235308412381234</c:v>
+                  <c:v>0.008899899328894824</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0004736619390710009</c:v>
+                  <c:v>0.007449022385713353</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.007769494006661343</c:v>
+                  <c:v>0.005613479187729091</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.006143419854082907</c:v>
+                  <c:v>-0.003571479312218215</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.01404733331097297</c:v>
+                  <c:v>-0.008772209685333602</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.009350888742858436</c:v>
+                  <c:v>0.005283362004705934</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.002076522824504694</c:v>
+                  <c:v>-0.001932949177437579</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.003753179370812564</c:v>
+                  <c:v>0.0006937044841925427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,22 +904,22 @@
         <v>-10</v>
       </c>
       <c r="B5">
-        <v>-0.004692317645432618</v>
+        <v>-0.003935650435941625</v>
       </c>
       <c r="C5">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D5">
-        <v>-0.004692317645432618</v>
+        <v>-0.003935650435941625</v>
       </c>
       <c r="E5">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="F5">
-        <v>-0.4637485706207821</v>
+        <v>-0.3118196591099094</v>
       </c>
       <c r="G5">
-        <v>0.3215826573229887</v>
+        <v>0.3776974515317684</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -927,22 +927,22 @@
         <v>-9</v>
       </c>
       <c r="B6">
-        <v>0.002273709198652002</v>
+        <v>0.009886099242211092</v>
       </c>
       <c r="C6">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D6">
-        <v>-0.002418608446780616</v>
+        <v>0.005950448806269467</v>
       </c>
       <c r="E6">
-        <v>0.0002047574137489418</v>
+        <v>0.0003186075373640478</v>
       </c>
       <c r="F6">
-        <v>-0.169022977351133</v>
+        <v>0.3333663041389559</v>
       </c>
       <c r="G6">
-        <v>0.4329464277467769</v>
+        <v>0.3695457225520961</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -950,22 +950,22 @@
         <v>-8</v>
       </c>
       <c r="B7">
-        <v>0.002968546493188109</v>
+        <v>0.03686949311152292</v>
       </c>
       <c r="C7">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D7">
-        <v>0.0005499380464074931</v>
+        <v>0.04281994191779238</v>
       </c>
       <c r="E7">
-        <v>0.0003071361206234127</v>
+        <v>0.0004779113060460718</v>
       </c>
       <c r="F7">
-        <v>0.03137966618747172</v>
+        <v>1.958720286988042</v>
       </c>
       <c r="G7">
-        <v>0.4874938464687534</v>
+        <v>0.02553743279552179</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -973,22 +973,22 @@
         <v>-7</v>
       </c>
       <c r="B8">
-        <v>-0.0005312292776401446</v>
+        <v>0.003929652349630477</v>
       </c>
       <c r="C8">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D8">
-        <v>1.870876876734848e-05</v>
+        <v>0.04674959426742286</v>
       </c>
       <c r="E8">
-        <v>0.0004095148274978836</v>
+        <v>0.0006372150747280957</v>
       </c>
       <c r="F8">
-        <v>0.0009245074001306953</v>
+        <v>1.851973744272164</v>
       </c>
       <c r="G8">
-        <v>0.4996314832149373</v>
+        <v>0.03250760010180109</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -996,22 +996,22 @@
         <v>-6</v>
       </c>
       <c r="B9">
-        <v>0.003876338607799104</v>
+        <v>-0.01491602802465154</v>
       </c>
       <c r="C9">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D9">
-        <v>0.003895047376566452</v>
+        <v>0.03183356624277132</v>
       </c>
       <c r="E9">
-        <v>0.0005118935343723546</v>
+        <v>0.0007965188434101196</v>
       </c>
       <c r="F9">
-        <v>0.1721563008929507</v>
+        <v>1.12794329553988</v>
       </c>
       <c r="G9">
-        <v>0.4317155582106158</v>
+        <v>0.1301240703682524</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1019,22 +1019,22 @@
         <v>-5</v>
       </c>
       <c r="B10">
-        <v>0.0257312630783711</v>
+        <v>-0.00794981979211278</v>
       </c>
       <c r="C10">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D10">
-        <v>0.02962631045493755</v>
+        <v>0.02388374645065854</v>
       </c>
       <c r="E10">
-        <v>0.0006142722412468254</v>
+        <v>0.0009558226120921435</v>
       </c>
       <c r="F10">
-        <v>1.195355610922904</v>
+        <v>0.7725272397247469</v>
       </c>
       <c r="G10">
-        <v>0.1164476627302201</v>
+        <v>0.2202062168233466</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1042,22 +1042,22 @@
         <v>-4</v>
       </c>
       <c r="B11">
-        <v>0.02487678499102481</v>
+        <v>-0.006848667889507258</v>
       </c>
       <c r="C11">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D11">
-        <v>0.05450309544596235</v>
+        <v>0.01703507856115128</v>
       </c>
       <c r="E11">
-        <v>0.0007166509481212963</v>
+        <v>0.001115126380774168</v>
       </c>
       <c r="F11">
-        <v>2.035951032472125</v>
+        <v>0.5101314461737966</v>
       </c>
       <c r="G11">
-        <v>0.02131824476720545</v>
+        <v>0.3051678688567327</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1065,22 +1065,22 @@
         <v>-3</v>
       </c>
       <c r="B12">
-        <v>0.01105313547977366</v>
+        <v>-0.009884378583264674</v>
       </c>
       <c r="C12">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D12">
-        <v>0.06555623092573601</v>
+        <v>0.007150699977886603</v>
       </c>
       <c r="E12">
-        <v>0.0008190296549957672</v>
+        <v>0.001274430149456191</v>
       </c>
       <c r="F12">
-        <v>2.290678623432303</v>
+        <v>0.2003044225103632</v>
       </c>
       <c r="G12">
-        <v>0.01133889088421769</v>
+        <v>0.4206893373338501</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1088,22 +1088,22 @@
         <v>-2</v>
       </c>
       <c r="B13">
-        <v>-0.01532719840851537</v>
+        <v>8.549523150954211e-05</v>
       </c>
       <c r="C13">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D13">
-        <v>0.05022903251722063</v>
+        <v>0.007236195209396145</v>
       </c>
       <c r="E13">
-        <v>0.0009214083618702382</v>
+        <v>0.001433733918138215</v>
       </c>
       <c r="F13">
-        <v>1.654736088053721</v>
+        <v>0.191106735737216</v>
       </c>
       <c r="G13">
-        <v>0.04951365702326749</v>
+        <v>0.4242858361062187</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1111,22 +1111,22 @@
         <v>-1</v>
       </c>
       <c r="B14">
-        <v>0.005706703300414887</v>
+        <v>-0.004063667302045998</v>
       </c>
       <c r="C14">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D14">
-        <v>0.05593573581763552</v>
+        <v>0.003172527907350148</v>
       </c>
       <c r="E14">
-        <v>0.001023787068744709</v>
+        <v>0.001593037686820239</v>
       </c>
       <c r="F14">
-        <v>1.74817351194436</v>
+        <v>0.07948632644739234</v>
       </c>
       <c r="G14">
-        <v>0.04073017772074672</v>
+        <v>0.4683494894655674</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1134,22 +1134,22 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>0.0212037115485405</v>
+        <v>0.000899859998840269</v>
       </c>
       <c r="C15">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D15">
-        <v>0.07713944736617602</v>
+        <v>0.004072387906190416</v>
       </c>
       <c r="E15">
-        <v>0.00112616577561918</v>
+        <v>0.001752341455502263</v>
       </c>
       <c r="F15">
-        <v>2.298663293313628</v>
+        <v>0.09728363091826903</v>
       </c>
       <c r="G15">
-        <v>0.01110684328579148</v>
+        <v>0.4612831664763337</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1157,22 +1157,22 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>0.007337797581017312</v>
+        <v>-0.009952276246002801</v>
       </c>
       <c r="C16">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D16">
-        <v>0.08447724494719333</v>
+        <v>-0.005879888339812385</v>
       </c>
       <c r="E16">
-        <v>0.001228544482493651</v>
+        <v>0.001911645224184287</v>
       </c>
       <c r="F16">
-        <v>2.410151256307123</v>
+        <v>-0.1344823937235355</v>
       </c>
       <c r="G16">
-        <v>0.008274765294570496</v>
+        <v>0.4465558055837257</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1180,22 +1180,22 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>0.002735197478940056</v>
+        <v>-0.01616381859091522</v>
       </c>
       <c r="C17">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D17">
-        <v>0.08721244242613338</v>
+        <v>-0.02204370693072761</v>
       </c>
       <c r="E17">
-        <v>0.001330923189368122</v>
+        <v>0.002070948992866311</v>
       </c>
       <c r="F17">
-        <v>2.390572686988324</v>
+        <v>-0.4843953074283416</v>
       </c>
       <c r="G17">
-        <v>0.008720392961795609</v>
+        <v>0.3142299889832101</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1203,22 +1203,22 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>0.005235308412381234</v>
+        <v>0.008899899328894824</v>
       </c>
       <c r="C18">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D18">
-        <v>0.09244775083851461</v>
+        <v>-0.01314380760183279</v>
       </c>
       <c r="E18">
-        <v>0.001433301896242593</v>
+        <v>0.002230252761548335</v>
       </c>
       <c r="F18">
-        <v>2.441897959448625</v>
+        <v>-0.278319829957595</v>
       </c>
       <c r="G18">
-        <v>0.007594819081439996</v>
+        <v>0.3904796133864255</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1226,22 +1226,22 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>0.0004736619390710009</v>
+        <v>0.007449022385713353</v>
       </c>
       <c r="C19">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D19">
-        <v>0.09292141277758562</v>
+        <v>-0.005694785216119432</v>
       </c>
       <c r="E19">
-        <v>0.001535680603117064</v>
+        <v>0.002389556530230359</v>
       </c>
       <c r="F19">
-        <v>2.37118454030007</v>
+        <v>-0.1164980602849768</v>
       </c>
       <c r="G19">
-        <v>0.009182392485772017</v>
+        <v>0.4536680156309918</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1249,22 +1249,22 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>-0.007769494006661343</v>
+        <v>0.005613479187729091</v>
       </c>
       <c r="C20">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D20">
-        <v>0.08515191877092428</v>
+        <v>-8.130602839034103e-05</v>
       </c>
       <c r="E20">
-        <v>0.001638059309991534</v>
+        <v>0.002548860298912383</v>
       </c>
       <c r="F20">
-        <v>2.103921963492323</v>
+        <v>-0.001610459215630958</v>
       </c>
       <c r="G20">
-        <v>0.01811007983901636</v>
+        <v>0.4993580569717858</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1272,22 +1272,22 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <v>-0.006143419854082907</v>
+        <v>-0.003571479312218215</v>
       </c>
       <c r="C21">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D21">
-        <v>0.07900849891684136</v>
+        <v>-0.003652785340608557</v>
       </c>
       <c r="E21">
-        <v>0.001740438016866005</v>
+        <v>0.002708164067594407</v>
       </c>
       <c r="F21">
-        <v>1.893845429320717</v>
+        <v>-0.07019184620400255</v>
       </c>
       <c r="G21">
-        <v>0.02960531652237697</v>
+        <v>0.4720439430898959</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1295,22 +1295,22 @@
         <v>7</v>
       </c>
       <c r="B22">
-        <v>-0.01404733331097297</v>
+        <v>-0.008772209685333602</v>
       </c>
       <c r="C22">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D22">
-        <v>0.0649611656058684</v>
+        <v>-0.01242499502594216</v>
       </c>
       <c r="E22">
-        <v>0.001842816723740476</v>
+        <v>0.00286746783627643</v>
       </c>
       <c r="F22">
-        <v>1.513257156543764</v>
+        <v>-0.2320314991130925</v>
       </c>
       <c r="G22">
-        <v>0.065635311009966</v>
+        <v>0.4083361375313432</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1318,22 +1318,22 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <v>-0.009350888742858436</v>
+        <v>0.005283362004705934</v>
       </c>
       <c r="C23">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D23">
-        <v>0.05561027686300996</v>
+        <v>-0.007141633021236225</v>
       </c>
       <c r="E23">
-        <v>0.001945195430614947</v>
+        <v>0.003026771604958455</v>
       </c>
       <c r="F23">
-        <v>1.26087907353337</v>
+        <v>-0.1298098668088332</v>
       </c>
       <c r="G23">
-        <v>0.1041676931111026</v>
+        <v>0.448402069746998</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1341,22 +1341,22 @@
         <v>9</v>
       </c>
       <c r="B24">
-        <v>0.002076522824504694</v>
+        <v>-0.001932949177437579</v>
       </c>
       <c r="C24">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D24">
-        <v>0.05768679968751465</v>
+        <v>-0.009074582198673804</v>
       </c>
       <c r="E24">
-        <v>0.002047574137489418</v>
+        <v>0.003186075373640478</v>
       </c>
       <c r="F24">
-        <v>1.274842779102422</v>
+        <v>-0.1607676323909191</v>
       </c>
       <c r="G24">
-        <v>0.1016773310975341</v>
+        <v>0.4361924923206937</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1364,22 +1364,22 @@
         <v>10</v>
       </c>
       <c r="B25">
-        <v>-0.003753179370812564</v>
+        <v>0.0006937044841925427</v>
       </c>
       <c r="C25">
-        <v>0.0001023787068744709</v>
+        <v>0.0001593037686820239</v>
       </c>
       <c r="D25">
-        <v>0.05393362031670209</v>
+        <v>-0.008380877714481261</v>
       </c>
       <c r="E25">
-        <v>0.002149952844363889</v>
+        <v>0.003345379142322502</v>
       </c>
       <c r="F25">
-        <v>1.163175125475308</v>
+        <v>-0.1448994815198182</v>
       </c>
       <c r="G25">
-        <v>0.1228429490610203</v>
+        <v>0.4424439297763026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>